<commit_message>
fixes exempted courses logic and makes general elective number of credits
</commit_message>
<xml_diff>
--- a/db/scrapper/src/csv/samples/Random Sample updated - Youssef 2.xlsx
+++ b/db/scrapper/src/csv/samples/Random Sample updated - Youssef 2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -1691,8 +1691,8 @@
   </sheetPr>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J29" activeCellId="0" sqref="J29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2183,11 +2183,11 @@
   </sheetPr>
   <dimension ref="A1:F1542"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J716" activeCellId="0" sqref="J716"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="8.54"/>
   </cols>
@@ -25836,7 +25836,7 @@
   </sheetPr>
   <dimension ref="A1:AE1866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A911" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A937" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>